<commit_message>
Scrutinizing Carnagey and Anderson 2005 entry.
</commit_message>
<xml_diff>
--- a/Craig_Table_2010.xlsx
+++ b/Craig_Table_2010.xlsx
@@ -3045,9 +3045,9 @@
   <dimension ref="A1:AJ481"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A237" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="O254" sqref="O254"/>
+      <selection pane="bottomLeft" activeCell="C468" sqref="C468"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -21407,7 +21407,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="232" spans="1:36">
+    <row r="232" spans="1:36" hidden="1">
       <c r="A232">
         <v>96</v>
       </c>
@@ -21484,7 +21484,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="233" spans="1:36">
+    <row r="233" spans="1:36" hidden="1">
       <c r="A233">
         <v>97</v>
       </c>
@@ -21792,7 +21792,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="237" spans="1:36" hidden="1">
+    <row r="237" spans="1:36">
       <c r="A237">
         <v>125</v>
       </c>
@@ -22212,26 +22212,26 @@
         <v>0.24955467004742601</v>
       </c>
       <c r="I242">
-        <f t="shared" ref="I242:I253" si="0">0.5*LN((1+G242)/(1-G242))</f>
+        <f>0.5*LN((1+G242)/(1-G242))</f>
         <v>6.8200544357650175E-2</v>
       </c>
       <c r="J242" s="3">
         <v>7.4300000000000005E-2</v>
       </c>
       <c r="K242">
-        <f t="shared" ref="K242:K263" si="1">1/SQRT(E242-3)</f>
+        <f>1/SQRT(E242-3)</f>
         <v>7.4329414624716636E-2</v>
       </c>
       <c r="L242">
-        <f t="shared" ref="L242:L248" si="2">I242/K242</f>
+        <f>I242/K242</f>
         <v>0.91754448359359964</v>
       </c>
       <c r="M242">
-        <f t="shared" ref="M242:M263" si="3">E242-2</f>
+        <f>E242-2</f>
         <v>182</v>
       </c>
       <c r="N242" t="e">
-        <f t="shared" ref="N242:N248" ca="1" si="4">_xlfn.T.DIST.2T(L242,M242)</f>
+        <f ca="1">_xlfn.T.DIST.2T(L242,M242)</f>
         <v>#NAME?</v>
       </c>
       <c r="O242" s="4" t="s">
@@ -22327,26 +22327,26 @@
         <v>0.190574089764425</v>
       </c>
       <c r="I243">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G243)/(1-G243))</f>
         <v>0.18715497016418453</v>
       </c>
       <c r="J243" s="1">
         <v>7.0534561585859801E-2</v>
       </c>
       <c r="K243">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E243-3)</f>
         <v>7.0534561585859828E-2</v>
       </c>
       <c r="L243">
-        <f t="shared" si="2"/>
+        <f>I243/K243</f>
         <v>2.6533796475982316</v>
       </c>
       <c r="M243">
-        <f t="shared" si="3"/>
+        <f>E243-2</f>
         <v>202</v>
       </c>
       <c r="N243" t="e">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">_xlfn.T.DIST.2T(L243,M243)</f>
         <v>#NAME?</v>
       </c>
       <c r="O243" s="4" t="s">
@@ -22442,26 +22442,26 @@
         <v>0.24912928181115701</v>
       </c>
       <c r="I244">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G244)/(1-G244))</f>
         <v>0.24668500792427897</v>
       </c>
       <c r="J244">
         <v>0.1</v>
       </c>
       <c r="K244">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E244-3)</f>
         <v>0.1</v>
       </c>
       <c r="L244">
-        <f t="shared" si="2"/>
+        <f>I244/K244</f>
         <v>2.4668500792427897</v>
       </c>
       <c r="M244">
-        <f t="shared" si="3"/>
+        <f>E244-2</f>
         <v>101</v>
       </c>
       <c r="N244" t="e">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">_xlfn.T.DIST.2T(L244,M244)</f>
         <v>#NAME?</v>
       </c>
       <c r="O244" s="4" t="s">
@@ -22554,26 +22554,26 @@
         <v>0.15984766512078499</v>
       </c>
       <c r="I245">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G245)/(1-G245))</f>
         <v>0.15697680915297069</v>
       </c>
       <c r="J245" s="1">
         <v>7.1981575074869505E-2</v>
       </c>
       <c r="K245">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E245-3)</f>
         <v>7.198157507486945E-2</v>
       </c>
       <c r="L245">
-        <f t="shared" si="2"/>
+        <f>I245/K245</f>
         <v>2.1807915288001967</v>
       </c>
       <c r="M245">
-        <f t="shared" si="3"/>
+        <f>E245-2</f>
         <v>194</v>
       </c>
       <c r="N245" t="e">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">_xlfn.T.DIST.2T(L245,M245)</f>
         <v>#NAME?</v>
       </c>
       <c r="O245" s="4" t="s">
@@ -22657,26 +22657,26 @@
         <v>0.10842286736361</v>
       </c>
       <c r="I246">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G246)/(1-G246))</f>
         <v>9.024418785614681E-2</v>
       </c>
       <c r="J246" s="1">
         <v>5.3376051268362402E-2</v>
       </c>
       <c r="K246">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E246-3)</f>
         <v>5.3376051268362382E-2</v>
       </c>
       <c r="L246">
-        <f t="shared" si="2"/>
+        <f>I246/K246</f>
         <v>1.6907243175861775</v>
       </c>
       <c r="M246">
-        <f t="shared" si="3"/>
+        <f>E246-2</f>
         <v>352</v>
       </c>
       <c r="N246" t="e">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">_xlfn.T.DIST.2T(L246,M246)</f>
         <v>#NAME?</v>
       </c>
       <c r="O246" s="5" t="s">
@@ -22766,26 +22766,26 @@
         <v>0.17413913148267501</v>
       </c>
       <c r="I247">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G247)/(1-G247))</f>
         <v>0.12058102840844412</v>
       </c>
       <c r="J247">
         <v>7.9555728417572996E-2</v>
       </c>
       <c r="K247">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E247-3)</f>
         <v>7.9555728417572996E-2</v>
       </c>
       <c r="L247">
-        <f t="shared" si="2"/>
+        <f>I247/K247</f>
         <v>1.5156800246430662</v>
       </c>
       <c r="M247">
-        <f t="shared" si="3"/>
+        <f>E247-2</f>
         <v>159</v>
       </c>
       <c r="N247" t="e">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">_xlfn.T.DIST.2T(L247,M247)</f>
         <v>#NAME?</v>
       </c>
       <c r="O247" s="5" t="s">
@@ -22875,26 +22875,26 @@
         <v>0.27664810875740697</v>
       </c>
       <c r="I248">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G248)/(1-G248))</f>
         <v>0.27470781051792986</v>
       </c>
       <c r="J248">
         <v>0.107211253483779</v>
       </c>
       <c r="K248">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E248-3)</f>
         <v>0.10721125348377948</v>
       </c>
       <c r="L248">
-        <f t="shared" si="2"/>
+        <f>I248/K248</f>
         <v>2.5623038775448301</v>
       </c>
       <c r="M248">
-        <f t="shared" si="3"/>
+        <f>E248-2</f>
         <v>88</v>
       </c>
       <c r="N248" t="e">
-        <f t="shared" ca="1" si="4"/>
+        <f ca="1">_xlfn.T.DIST.2T(L248,M248)</f>
         <v>#NAME?</v>
       </c>
       <c r="O248" s="4" t="s">
@@ -22984,21 +22984,21 @@
         <v>0.39912496552020998</v>
       </c>
       <c r="I249" t="e">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G249)/(1-G249))</f>
         <v>#VALUE!</v>
       </c>
       <c r="J249">
         <v>0.242535625036333</v>
       </c>
       <c r="K249">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E249-3)</f>
         <v>0.24253562503633297</v>
       </c>
       <c r="L249" t="s">
         <v>795</v>
       </c>
       <c r="M249">
-        <f t="shared" si="3"/>
+        <f>E249-2</f>
         <v>18</v>
       </c>
       <c r="N249" t="s">
@@ -23091,21 +23091,21 @@
         <v>0.64250092791544</v>
       </c>
       <c r="I250" t="e">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G250)/(1-G250))</f>
         <v>#VALUE!</v>
       </c>
       <c r="J250">
         <v>0.25</v>
       </c>
       <c r="K250">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E250-3)</f>
         <v>0.25</v>
       </c>
       <c r="L250" t="s">
         <v>795</v>
       </c>
       <c r="M250">
-        <f t="shared" si="3"/>
+        <f>E250-2</f>
         <v>17</v>
       </c>
       <c r="N250" t="s">
@@ -23195,14 +23195,14 @@
         <v>0.48509999999999998</v>
       </c>
       <c r="I251">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G251)/(1-G251))</f>
         <v>0.52963234099240197</v>
       </c>
       <c r="J251">
         <v>0.16669999999999999</v>
       </c>
       <c r="K251">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E251-3)</f>
         <v>0.16666666666666666</v>
       </c>
       <c r="L251">
@@ -23210,7 +23210,7 @@
         <v>3.1777940459544118</v>
       </c>
       <c r="M251">
-        <f t="shared" si="3"/>
+        <f>E251-2</f>
         <v>37</v>
       </c>
       <c r="N251" t="e">
@@ -23307,14 +23307,14 @@
         <v>0.39655798997060099</v>
       </c>
       <c r="I252">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G252)/(1-G252))</f>
         <v>0.39772417941721228</v>
       </c>
       <c r="J252">
         <v>0.115470053837925</v>
       </c>
       <c r="K252">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E252-3)</f>
         <v>0.11470786693528087</v>
       </c>
       <c r="L252">
@@ -23322,7 +23322,7 @@
         <v>3.4672790109645359</v>
       </c>
       <c r="M252">
-        <f t="shared" si="3"/>
+        <f>E252-2</f>
         <v>77</v>
       </c>
       <c r="N252" t="e">
@@ -23422,14 +23422,14 @@
         <v>0.21840781899612</v>
       </c>
       <c r="I253">
-        <f t="shared" si="0"/>
+        <f>0.5*LN((1+G253)/(1-G253))</f>
         <v>7.6549170686205217E-2</v>
       </c>
       <c r="J253" s="1">
         <v>9.4491118252306799E-2</v>
       </c>
       <c r="K253">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E253-3)</f>
         <v>9.284766908852593E-2</v>
       </c>
       <c r="L253">
@@ -23437,7 +23437,7 @@
         <v>0.82445979998936914</v>
       </c>
       <c r="M253">
-        <f t="shared" si="3"/>
+        <f>E253-2</f>
         <v>117</v>
       </c>
       <c r="N253" t="e">
@@ -23508,7 +23508,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="254" spans="1:36" ht="15.75">
+    <row r="254" spans="1:36" ht="15.75" hidden="1">
       <c r="A254">
         <v>98</v>
       </c>
@@ -23540,14 +23540,14 @@
         <v>0.145864991497895</v>
       </c>
       <c r="K254">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E254-3)</f>
         <v>0.14586499149789456</v>
       </c>
       <c r="L254" t="s">
         <v>795</v>
       </c>
       <c r="M254">
-        <f t="shared" si="3"/>
+        <f>E254-2</f>
         <v>48</v>
       </c>
       <c r="N254" t="s">
@@ -23608,7 +23608,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="255" spans="1:36" ht="15.75">
+    <row r="255" spans="1:36" ht="15.75" hidden="1">
       <c r="A255">
         <v>99</v>
       </c>
@@ -23640,14 +23640,14 @@
         <v>0.145864991497895</v>
       </c>
       <c r="K255">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E255-3)</f>
         <v>0.14586499149789456</v>
       </c>
       <c r="L255" t="s">
         <v>795</v>
       </c>
       <c r="M255">
-        <f t="shared" si="3"/>
+        <f>E255-2</f>
         <v>48</v>
       </c>
       <c r="N255" t="s">
@@ -23711,7 +23711,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="256" spans="1:36" ht="15.75">
+    <row r="256" spans="1:36" ht="15.75" hidden="1">
       <c r="B256" t="s">
         <v>804</v>
       </c>
@@ -23739,19 +23739,19 @@
         <v>0.10150000000000001</v>
       </c>
       <c r="K256">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E256-3)</f>
         <v>0.10153461651336192</v>
       </c>
       <c r="L256">
-        <f t="shared" ref="L256:L263" si="5">I256/K256</f>
+        <f>I256/K256</f>
         <v>2.0994942797347003</v>
       </c>
       <c r="M256">
-        <f t="shared" si="3"/>
+        <f>E256-2</f>
         <v>98</v>
       </c>
       <c r="N256" t="e">
-        <f t="shared" ref="N256:N263" ca="1" si="6">_xlfn.T.DIST.2T(L256,M256)</f>
+        <f ca="1">_xlfn.T.DIST.2T(L256,M256)</f>
         <v>#NAME?</v>
       </c>
       <c r="O256" s="4" t="s">
@@ -23848,19 +23848,19 @@
         <v>0.117041147196131</v>
       </c>
       <c r="K257">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E257-3)</f>
         <v>0.11704114719613057</v>
       </c>
       <c r="L257">
-        <f t="shared" si="5"/>
+        <f>I257/K257</f>
         <v>2.2736312249889821</v>
       </c>
       <c r="M257">
-        <f t="shared" si="3"/>
+        <f>E257-2</f>
         <v>74</v>
       </c>
       <c r="N257" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">_xlfn.T.DIST.2T(L257,M257)</f>
         <v>#NAME?</v>
       </c>
       <c r="O257" s="4" t="s">
@@ -23924,65 +23924,46 @@
         <v>774</v>
       </c>
     </row>
-    <row r="258" spans="1:36" ht="15.75" hidden="1">
+    <row r="258" spans="1:36">
       <c r="A258">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B258" t="s">
-        <v>513</v>
+        <v>507</v>
       </c>
       <c r="C258" t="s">
         <v>737</v>
       </c>
       <c r="D258" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="E258" s="2">
-        <v>90</v>
-      </c>
-      <c r="F258" s="4">
-        <v>0.21490000000000001</v>
-      </c>
-      <c r="G258" s="4">
-        <v>0.21129999999999999</v>
+        <v>141</v>
+      </c>
+      <c r="F258">
+        <v>0.32700000000000001</v>
       </c>
       <c r="H258">
-        <v>0.21830297482824301</v>
-      </c>
-      <c r="I258">
-        <f>0.5*LN((1+G258)/(1-G258))</f>
-        <v>0.2145317108094057</v>
-      </c>
-      <c r="J258">
-        <v>0.107211253483779</v>
-      </c>
-      <c r="K258">
-        <f t="shared" si="1"/>
-        <v>0.10721125348377948</v>
-      </c>
-      <c r="L258">
-        <f t="shared" si="5"/>
-        <v>2.0010185856269582</v>
-      </c>
-      <c r="M258">
-        <f t="shared" si="3"/>
-        <v>88</v>
-      </c>
-      <c r="N258" t="e">
-        <f t="shared" ca="1" si="6"/>
-        <v>#NAME?</v>
-      </c>
-      <c r="O258" s="4" t="s">
+        <v>0.33946535234373998</v>
+      </c>
+      <c r="J258" s="1">
+        <v>8.5125653075874899E-2</v>
+      </c>
+      <c r="K258" s="1"/>
+      <c r="L258" s="1"/>
+      <c r="M258" s="1"/>
+      <c r="N258" s="1"/>
+      <c r="O258" t="s">
         <v>506</v>
       </c>
       <c r="P258" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="Q258" t="s">
         <v>727</v>
       </c>
       <c r="R258">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="S258" t="s">
         <v>729</v>
@@ -23990,9 +23971,6 @@
       <c r="T258" t="s">
         <v>727</v>
       </c>
-      <c r="U258" t="s">
-        <v>727</v>
-      </c>
       <c r="V258" t="s">
         <v>731</v>
       </c>
@@ -24000,10 +23978,10 @@
         <v>732</v>
       </c>
       <c r="X258" t="s">
-        <v>730</v>
+        <v>751</v>
       </c>
       <c r="Y258" t="s">
-        <v>730</v>
+        <v>751</v>
       </c>
       <c r="Z258" t="s">
         <v>733</v>
@@ -24018,22 +23996,13 @@
         <v>733</v>
       </c>
       <c r="AD258">
-        <v>0.21490000000000001</v>
+        <v>0.34</v>
       </c>
       <c r="AE258" t="s">
         <v>733</v>
       </c>
       <c r="AF258" t="s">
         <v>735</v>
-      </c>
-      <c r="AH258" t="s">
-        <v>775</v>
-      </c>
-      <c r="AI258">
-        <v>1.1900000000000001E-2</v>
-      </c>
-      <c r="AJ258" t="s">
-        <v>776</v>
       </c>
     </row>
     <row r="259" spans="1:36" ht="15.75" hidden="1">
@@ -24069,19 +24038,19 @@
         <v>0.128036879932896</v>
       </c>
       <c r="K259">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E259-3)</f>
         <v>0.12803687993289598</v>
       </c>
       <c r="L259">
-        <f t="shared" si="5"/>
+        <f>I259/K259</f>
         <v>1.4698156255931552</v>
       </c>
       <c r="M259">
-        <f t="shared" si="3"/>
+        <f>E259-2</f>
         <v>62</v>
       </c>
       <c r="N259" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">_xlfn.T.DIST.2T(L259,M259)</f>
         <v>#NAME?</v>
       </c>
       <c r="O259" s="4" t="s">
@@ -24181,19 +24150,19 @@
         <v>7.9555728417572996E-2</v>
       </c>
       <c r="K260">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E260-3)</f>
         <v>7.9555728417572996E-2</v>
       </c>
       <c r="L260">
-        <f t="shared" si="5"/>
+        <f>I260/K260</f>
         <v>2.9516802455953348</v>
       </c>
       <c r="M260">
-        <f t="shared" si="3"/>
+        <f>E260-2</f>
         <v>159</v>
       </c>
       <c r="N260" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">_xlfn.T.DIST.2T(L260,M260)</f>
         <v>#NAME?</v>
       </c>
       <c r="O260" s="12" t="s">
@@ -24290,19 +24259,19 @@
         <v>0.132453235706504</v>
       </c>
       <c r="K261">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E261-3)</f>
         <v>0.13245323570650439</v>
       </c>
       <c r="L261">
-        <f t="shared" si="5"/>
+        <f>I261/K261</f>
         <v>2.3950328999141322</v>
       </c>
       <c r="M261">
-        <f t="shared" si="3"/>
+        <f>E261-2</f>
         <v>58</v>
       </c>
       <c r="N261" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">_xlfn.T.DIST.2T(L261,M261)</f>
         <v>#NAME?</v>
       </c>
       <c r="O261" s="8" t="s">
@@ -24393,19 +24362,19 @@
         <v>0.14907119849998601</v>
       </c>
       <c r="K262">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E262-3)</f>
         <v>0.14907119849998599</v>
       </c>
       <c r="L262">
-        <f t="shared" si="5"/>
+        <f>I262/K262</f>
         <v>2.1673667082528731</v>
       </c>
       <c r="M262">
-        <f t="shared" si="3"/>
+        <f>E262-2</f>
         <v>46</v>
       </c>
       <c r="N262" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">_xlfn.T.DIST.2T(L262,M262)</f>
         <v>#NAME?</v>
       </c>
       <c r="O262" s="6" t="s">
@@ -24499,19 +24468,19 @@
         <v>0.18898223650461399</v>
       </c>
       <c r="K263">
-        <f t="shared" si="1"/>
+        <f>1/SQRT(E263-3)</f>
         <v>0.1889822365046136</v>
       </c>
       <c r="L263">
-        <f t="shared" si="5"/>
+        <f>I263/K263</f>
         <v>1.6786226212822644</v>
       </c>
       <c r="M263">
-        <f t="shared" si="3"/>
+        <f>E263-2</f>
         <v>29</v>
       </c>
       <c r="N263" t="e">
-        <f t="shared" ca="1" si="6"/>
+        <f ca="1">_xlfn.T.DIST.2T(L263,M263)</f>
         <v>#NAME?</v>
       </c>
       <c r="O263" s="6" t="s">
@@ -25286,45 +25255,45 @@
         <v>735</v>
       </c>
     </row>
-    <row r="273" spans="1:36" hidden="1">
+    <row r="273" spans="1:36">
       <c r="A273">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B273" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="C273" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="D273" t="s">
-        <v>724</v>
+        <v>733</v>
       </c>
       <c r="E273" s="2">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="F273">
-        <v>0.38329999999999997</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="H273">
-        <v>0.403922272941661</v>
+        <v>0.136847915238521</v>
       </c>
       <c r="J273">
-        <v>0.15617376188860599</v>
+        <v>0.120385853085769</v>
       </c>
       <c r="O273" t="s">
         <v>506</v>
       </c>
       <c r="P273" t="s">
-        <v>730</v>
+        <v>734</v>
       </c>
       <c r="Q273" t="s">
         <v>727</v>
       </c>
       <c r="R273">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S273" t="s">
-        <v>729</v>
+        <v>681</v>
       </c>
       <c r="T273" t="s">
         <v>727</v>
@@ -25336,10 +25305,10 @@
         <v>732</v>
       </c>
       <c r="X273" t="s">
-        <v>730</v>
+        <v>751</v>
       </c>
       <c r="Y273" t="s">
-        <v>730</v>
+        <v>662</v>
       </c>
       <c r="Z273" t="s">
         <v>733</v>
@@ -25354,7 +25323,7 @@
         <v>733</v>
       </c>
       <c r="AD273">
-        <v>0.38329999999999997</v>
+        <v>0.13600000000000001</v>
       </c>
       <c r="AE273" t="s">
         <v>733</v>
@@ -26404,7 +26373,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="287" spans="1:36">
+    <row r="287" spans="1:36" hidden="1">
       <c r="A287">
         <v>102</v>
       </c>
@@ -26482,7 +26451,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="288" spans="1:36">
+    <row r="288" spans="1:36" hidden="1">
       <c r="A288">
         <v>103</v>
       </c>
@@ -29898,7 +29867,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="331" spans="1:32">
+    <row r="331" spans="1:32" hidden="1">
       <c r="A331">
         <v>75</v>
       </c>
@@ -30694,12 +30663,12 @@
         <v>489</v>
       </c>
     </row>
-    <row r="341" spans="1:32" hidden="1">
+    <row r="341" spans="1:32">
       <c r="A341">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B341" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C341" t="s">
         <v>737</v>
@@ -30708,21 +30677,17 @@
         <v>733</v>
       </c>
       <c r="E341" s="2">
-        <v>141</v>
+        <v>69</v>
       </c>
       <c r="F341">
-        <v>0.32700000000000001</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="H341">
-        <v>0.33946535234373998</v>
-      </c>
-      <c r="J341" s="1">
-        <v>8.5125653075874899E-2</v>
-      </c>
-      <c r="K341" s="1"/>
-      <c r="L341" s="1"/>
-      <c r="M341" s="1"/>
-      <c r="N341" s="1"/>
+        <v>0.14705085174305699</v>
+      </c>
+      <c r="J341">
+        <v>0.123091490979333</v>
+      </c>
       <c r="O341" t="s">
         <v>506</v>
       </c>
@@ -30736,7 +30701,7 @@
         <v>1</v>
       </c>
       <c r="S341" t="s">
-        <v>729</v>
+        <v>679</v>
       </c>
       <c r="T341" t="s">
         <v>727</v>
@@ -30751,7 +30716,7 @@
         <v>751</v>
       </c>
       <c r="Y341" t="s">
-        <v>751</v>
+        <v>662</v>
       </c>
       <c r="Z341" t="s">
         <v>733</v>
@@ -30766,7 +30731,7 @@
         <v>733</v>
       </c>
       <c r="AD341">
-        <v>0.34</v>
+        <v>0.14599999999999999</v>
       </c>
       <c r="AE341" t="s">
         <v>733</v>
@@ -30933,46 +30898,42 @@
         <v>33</v>
       </c>
     </row>
-    <row r="344" spans="1:32" hidden="1">
+    <row r="344" spans="1:32">
       <c r="A344">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="B344" t="s">
-        <v>510</v>
+        <v>514</v>
       </c>
       <c r="C344" t="s">
-        <v>737</v>
+        <v>743</v>
       </c>
       <c r="D344" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="E344" s="2">
-        <v>135</v>
+        <v>44</v>
       </c>
       <c r="F344">
-        <v>0.23</v>
+        <v>0.38329999999999997</v>
       </c>
       <c r="H344">
-        <v>0.234189466759367</v>
-      </c>
-      <c r="J344" s="1">
-        <v>8.7038827977848898E-2</v>
-      </c>
-      <c r="K344" s="1"/>
-      <c r="L344" s="1"/>
-      <c r="M344" s="1"/>
-      <c r="N344" s="1"/>
+        <v>0.403922272941661</v>
+      </c>
+      <c r="J344">
+        <v>0.15617376188860599</v>
+      </c>
       <c r="O344" t="s">
         <v>506</v>
       </c>
       <c r="P344" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="Q344" t="s">
         <v>727</v>
       </c>
       <c r="R344">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S344" t="s">
         <v>729</v>
@@ -30987,10 +30948,10 @@
         <v>732</v>
       </c>
       <c r="X344" t="s">
-        <v>751</v>
+        <v>730</v>
       </c>
       <c r="Y344" t="s">
-        <v>751</v>
+        <v>730</v>
       </c>
       <c r="Z344" t="s">
         <v>733</v>
@@ -31005,7 +30966,7 @@
         <v>733</v>
       </c>
       <c r="AD344">
-        <v>0.23</v>
+        <v>0.38329999999999997</v>
       </c>
       <c r="AE344" t="s">
         <v>733</v>
@@ -34228,7 +34189,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="385" spans="1:36">
+    <row r="385" spans="1:36" hidden="1">
       <c r="A385">
         <v>70</v>
       </c>
@@ -35090,7 +35051,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="396" spans="1:36" ht="15.75">
+    <row r="396" spans="1:36" ht="15.75" hidden="1">
       <c r="A396">
         <v>71</v>
       </c>
@@ -36197,7 +36158,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="410" spans="1:36">
+    <row r="410" spans="1:36" hidden="1">
       <c r="A410">
         <v>72</v>
       </c>
@@ -36351,7 +36312,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="412" spans="1:36">
+    <row r="412" spans="1:36" hidden="1">
       <c r="A412">
         <v>100</v>
       </c>
@@ -36428,7 +36389,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="413" spans="1:36">
+    <row r="413" spans="1:36" hidden="1">
       <c r="A413">
         <v>101</v>
       </c>
@@ -38609,7 +38570,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="441" spans="1:36">
+    <row r="441" spans="1:36" hidden="1">
       <c r="A441">
         <v>73</v>
       </c>
@@ -40484,7 +40445,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="465" spans="1:32" hidden="1">
+    <row r="465" spans="1:36" hidden="1">
       <c r="A465">
         <v>21</v>
       </c>
@@ -40561,7 +40522,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="466" spans="1:32" hidden="1">
+    <row r="466" spans="1:36" hidden="1">
       <c r="A466">
         <v>43</v>
       </c>
@@ -40638,47 +40599,73 @@
         <v>735</v>
       </c>
     </row>
-    <row r="467" spans="1:32" hidden="1">
+    <row r="467" spans="1:36" ht="15.75">
       <c r="A467">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="B467" t="s">
-        <v>509</v>
+        <v>513</v>
       </c>
       <c r="C467" t="s">
         <v>737</v>
       </c>
       <c r="D467" t="s">
-        <v>733</v>
+        <v>724</v>
       </c>
       <c r="E467" s="2">
-        <v>72</v>
-      </c>
-      <c r="F467">
-        <v>0.13600000000000001</v>
+        <v>90</v>
+      </c>
+      <c r="F467" s="4">
+        <v>0.21490000000000001</v>
+      </c>
+      <c r="G467" s="4">
+        <v>0.21129999999999999</v>
       </c>
       <c r="H467">
-        <v>0.136847915238521</v>
+        <v>0.21830297482824301</v>
+      </c>
+      <c r="I467">
+        <f>0.5*LN((1+G467)/(1-G467))</f>
+        <v>0.2145317108094057</v>
       </c>
       <c r="J467">
-        <v>0.120385853085769</v>
-      </c>
-      <c r="O467" t="s">
+        <v>0.107211253483779</v>
+      </c>
+      <c r="K467">
+        <f>1/SQRT(E467-3)</f>
+        <v>0.10721125348377948</v>
+      </c>
+      <c r="L467">
+        <f>I467/K467</f>
+        <v>2.0010185856269582</v>
+      </c>
+      <c r="M467">
+        <f>E467-2</f>
+        <v>88</v>
+      </c>
+      <c r="N467" t="e">
+        <f ca="1">_xlfn.T.DIST.2T(L467,M467)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="O467" s="4" t="s">
         <v>506</v>
       </c>
       <c r="P467" t="s">
-        <v>734</v>
+        <v>730</v>
       </c>
       <c r="Q467" t="s">
         <v>727</v>
       </c>
       <c r="R467">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S467" t="s">
-        <v>681</v>
+        <v>729</v>
       </c>
       <c r="T467" t="s">
+        <v>727</v>
+      </c>
+      <c r="U467" t="s">
         <v>727</v>
       </c>
       <c r="V467" t="s">
@@ -40688,10 +40675,10 @@
         <v>732</v>
       </c>
       <c r="X467" t="s">
-        <v>751</v>
+        <v>730</v>
       </c>
       <c r="Y467" t="s">
-        <v>662</v>
+        <v>730</v>
       </c>
       <c r="Z467" t="s">
         <v>733</v>
@@ -40706,7 +40693,7 @@
         <v>733</v>
       </c>
       <c r="AD467">
-        <v>0.13600000000000001</v>
+        <v>0.21490000000000001</v>
       </c>
       <c r="AE467" t="s">
         <v>733</v>
@@ -40714,13 +40701,22 @@
       <c r="AF467" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="468" spans="1:32" hidden="1">
+      <c r="AH467" t="s">
+        <v>775</v>
+      </c>
+      <c r="AI467">
+        <v>1.1900000000000001E-2</v>
+      </c>
+      <c r="AJ467" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="468" spans="1:36">
       <c r="A468">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B468" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="C468" t="s">
         <v>737</v>
@@ -40729,17 +40725,21 @@
         <v>733</v>
       </c>
       <c r="E468" s="2">
-        <v>72</v>
+        <v>135</v>
       </c>
       <c r="F468">
-        <v>0.14399999999999999</v>
+        <v>0.23</v>
       </c>
       <c r="H468">
-        <v>0.14500789789900101</v>
-      </c>
-      <c r="J468">
-        <v>0.120385853085769</v>
-      </c>
+        <v>0.234189466759367</v>
+      </c>
+      <c r="J468" s="1">
+        <v>8.7038827977848898E-2</v>
+      </c>
+      <c r="K468" s="1"/>
+      <c r="L468" s="1"/>
+      <c r="M468" s="1"/>
+      <c r="N468" s="1"/>
       <c r="O468" t="s">
         <v>506</v>
       </c>
@@ -40753,7 +40753,7 @@
         <v>3</v>
       </c>
       <c r="S468" t="s">
-        <v>679</v>
+        <v>729</v>
       </c>
       <c r="T468" t="s">
         <v>727</v>
@@ -40768,7 +40768,7 @@
         <v>751</v>
       </c>
       <c r="Y468" t="s">
-        <v>662</v>
+        <v>751</v>
       </c>
       <c r="Z468" t="s">
         <v>733</v>
@@ -40783,7 +40783,7 @@
         <v>733</v>
       </c>
       <c r="AD468">
-        <v>0.14399999999999999</v>
+        <v>0.23</v>
       </c>
       <c r="AE468" t="s">
         <v>733</v>
@@ -40792,12 +40792,12 @@
         <v>735</v>
       </c>
     </row>
-    <row r="469" spans="1:32" hidden="1">
+    <row r="469" spans="1:36">
       <c r="A469">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B469" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="C469" t="s">
         <v>737</v>
@@ -40806,16 +40806,16 @@
         <v>733</v>
       </c>
       <c r="E469" s="2">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="F469">
-        <v>0.14599999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="H469">
-        <v>0.14705085174305699</v>
+        <v>0.14500789789900101</v>
       </c>
       <c r="J469">
-        <v>0.123091490979333</v>
+        <v>0.120385853085769</v>
       </c>
       <c r="O469" t="s">
         <v>506</v>
@@ -40827,7 +40827,7 @@
         <v>727</v>
       </c>
       <c r="R469">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="S469" t="s">
         <v>679</v>
@@ -40860,7 +40860,7 @@
         <v>733</v>
       </c>
       <c r="AD469">
-        <v>0.14599999999999999</v>
+        <v>0.14399999999999999</v>
       </c>
       <c r="AE469" t="s">
         <v>733</v>
@@ -40869,7 +40869,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="470" spans="1:32" hidden="1">
+    <row r="470" spans="1:36">
       <c r="A470">
         <v>131</v>
       </c>
@@ -40947,7 +40947,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="471" spans="1:32" hidden="1">
+    <row r="471" spans="1:36" hidden="1">
       <c r="A471">
         <v>261</v>
       </c>
@@ -41024,7 +41024,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="472" spans="1:32" hidden="1">
+    <row r="472" spans="1:36" hidden="1">
       <c r="A472">
         <v>192</v>
       </c>
@@ -41101,7 +41101,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="473" spans="1:32" hidden="1">
+    <row r="473" spans="1:36" hidden="1">
       <c r="A473">
         <v>88</v>
       </c>
@@ -41178,7 +41178,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="474" spans="1:32" hidden="1">
+    <row r="474" spans="1:36" hidden="1">
       <c r="A474">
         <v>187</v>
       </c>
@@ -41255,7 +41255,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="475" spans="1:32">
+    <row r="475" spans="1:36" hidden="1">
       <c r="A475">
         <v>76</v>
       </c>
@@ -41337,7 +41337,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="476" spans="1:32" hidden="1">
+    <row r="476" spans="1:36" hidden="1">
       <c r="A476">
         <v>150</v>
       </c>
@@ -41419,7 +41419,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="477" spans="1:32" hidden="1">
+    <row r="477" spans="1:36" hidden="1">
       <c r="A477">
         <v>151</v>
       </c>
@@ -41501,7 +41501,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="478" spans="1:32" hidden="1">
+    <row r="478" spans="1:36" hidden="1">
       <c r="A478">
         <v>202</v>
       </c>
@@ -41578,7 +41578,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="479" spans="1:32" hidden="1">
+    <row r="479" spans="1:36" hidden="1">
       <c r="A479">
         <v>203</v>
       </c>
@@ -41660,7 +41660,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="480" spans="1:32" hidden="1">
+    <row r="480" spans="1:36" hidden="1">
       <c r="A480">
         <v>305</v>
       </c>
@@ -41747,14 +41747,14 @@
   <autoFilter ref="A1:AJ481">
     <filterColumn colId="2"/>
     <filterColumn colId="14">
-      <customFilters>
-        <customFilter val="*Brady*"/>
-      </customFilters>
+      <filters>
+        <filter val="Carnagey, N. L., &amp; Anderson, C.A. (2005). The effects of reward and punishment in violent video games on aggressive affect, cognition, and behavior. Psychological Science, 16, 882-889."/>
+      </filters>
     </filterColumn>
     <filterColumn colId="15"/>
     <filterColumn colId="24"/>
-    <sortState ref="A5:AJ474">
-      <sortCondition descending="1" ref="E1:E481"/>
+    <sortState ref="A237:AJ470">
+      <sortCondition ref="R1:R481"/>
     </sortState>
   </autoFilter>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>